<commit_message>
Refined output formatting and improved data presentation for final report
</commit_message>
<xml_diff>
--- a/data/results.xlsx
+++ b/data/results.xlsx
@@ -295,7 +295,7 @@
         <v>12</v>
       </c>
       <c r="J2" t="n" s="0">
-        <v>2.7359</v>
+        <v>2.6862</v>
       </c>
     </row>
     <row r="3">
@@ -327,7 +327,7 @@
         <v>16</v>
       </c>
       <c r="J3" t="n" s="0">
-        <v>1.8424</v>
+        <v>3.0631</v>
       </c>
     </row>
     <row r="4">
@@ -359,7 +359,7 @@
         <v>22</v>
       </c>
       <c r="J4" t="n" s="0">
-        <v>2.4323</v>
+        <v>2.2513</v>
       </c>
     </row>
     <row r="5">
@@ -391,7 +391,7 @@
         <v>27</v>
       </c>
       <c r="J5" t="n" s="0">
-        <v>2.0534</v>
+        <v>2.9341</v>
       </c>
     </row>
     <row r="6">
@@ -423,7 +423,7 @@
         <v>30</v>
       </c>
       <c r="J6" t="n" s="0">
-        <v>1.8871</v>
+        <v>1.5682</v>
       </c>
     </row>
     <row r="7">
@@ -455,7 +455,7 @@
         <v>33</v>
       </c>
       <c r="J7" t="n" s="0">
-        <v>1.5848</v>
+        <v>2.2149</v>
       </c>
     </row>
     <row r="8">
@@ -487,7 +487,7 @@
         <v>33</v>
       </c>
       <c r="J8" t="n" s="0">
-        <v>2.7659</v>
+        <v>3.0488</v>
       </c>
     </row>
     <row r="9">
@@ -519,7 +519,7 @@
         <v>40</v>
       </c>
       <c r="J9" t="n" s="0">
-        <v>4.5589</v>
+        <v>2.391</v>
       </c>
     </row>
     <row r="10">
@@ -551,7 +551,7 @@
         <v>43</v>
       </c>
       <c r="J10" t="n" s="0">
-        <v>3.1594</v>
+        <v>3.3008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>